<commit_message>
add dx score comparison without relapse samples
</commit_message>
<xml_diff>
--- a/data/tableone_Dx_pacmap.xlsx
+++ b/data/tableone_Dx_pacmap.xlsx
@@ -106,76 +106,76 @@
     <t>TCGA AML</t>
   </si>
   <si>
-    <t>905 (38.0)</t>
-  </si>
-  <si>
-    <t>1107 (46.5)</t>
-  </si>
-  <si>
-    <t>31 (1.3)</t>
-  </si>
-  <si>
-    <t>51 (2.1)</t>
-  </si>
-  <si>
-    <t>147 (6.2)</t>
-  </si>
-  <si>
-    <t>140 (5.9)</t>
-  </si>
-  <si>
-    <t>480 (24.1)</t>
-  </si>
-  <si>
-    <t>482 (24.2)</t>
-  </si>
-  <si>
-    <t>658 (33.1)</t>
-  </si>
-  <si>
-    <t>165 (8.3)</t>
-  </si>
-  <si>
-    <t>203 (10.2)</t>
-  </si>
-  <si>
-    <t>883 (49.1)</t>
-  </si>
-  <si>
-    <t>914 (50.9)</t>
-  </si>
-  <si>
-    <t>72 (2.4)</t>
-  </si>
-  <si>
-    <t>628 (20.5)</t>
-  </si>
-  <si>
-    <t>581 (19.0)</t>
-  </si>
-  <si>
-    <t>316 (10.3)</t>
-  </si>
-  <si>
-    <t>41 (1.3)</t>
-  </si>
-  <si>
-    <t>83 (2.7)</t>
-  </si>
-  <si>
-    <t>153 (5.0)</t>
-  </si>
-  <si>
-    <t>64 (2.1)</t>
-  </si>
-  <si>
-    <t>796 (26.0)</t>
-  </si>
-  <si>
-    <t>131 (4.3)</t>
-  </si>
-  <si>
-    <t>194 (6.3)</t>
+    <t>905 (41.8)</t>
+  </si>
+  <si>
+    <t>902 (41.7)</t>
+  </si>
+  <si>
+    <t>31 (1.4)</t>
+  </si>
+  <si>
+    <t>48 (2.2)</t>
+  </si>
+  <si>
+    <t>138 (6.4)</t>
+  </si>
+  <si>
+    <t>140 (6.5)</t>
+  </si>
+  <si>
+    <t>398 (22.9)</t>
+  </si>
+  <si>
+    <t>395 (22.7)</t>
+  </si>
+  <si>
+    <t>576 (33.2)</t>
+  </si>
+  <si>
+    <t>165 (9.5)</t>
+  </si>
+  <si>
+    <t>203 (11.7)</t>
+  </si>
+  <si>
+    <t>766 (49.5)</t>
+  </si>
+  <si>
+    <t>783 (50.5)</t>
+  </si>
+  <si>
+    <t>58 (2.1)</t>
+  </si>
+  <si>
+    <t>592 (21.6)</t>
+  </si>
+  <si>
+    <t>397 (14.5)</t>
+  </si>
+  <si>
+    <t>280 (10.2)</t>
+  </si>
+  <si>
+    <t>27 (1.0)</t>
+  </si>
+  <si>
+    <t>83 (3.0)</t>
+  </si>
+  <si>
+    <t>153 (5.6)</t>
+  </si>
+  <si>
+    <t>64 (2.3)</t>
+  </si>
+  <si>
+    <t>764 (27.9)</t>
+  </si>
+  <si>
+    <t>128 (4.7)</t>
+  </si>
+  <si>
+    <t>194 (7.1)</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2">
-        <v>3059</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>